<commit_message>
Next use of TRIMRANGE
</commit_message>
<xml_diff>
--- a/TrimRangeDrill.xlsx
+++ b/TrimRangeDrill.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{E4E3595A-9E4B-4617-8E8E-2C1CB2528D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299DDB0B-FAAE-4A3C-88AA-4454D4B1864E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstDrill" sheetId="1" r:id="rId1"/>
+    <sheet name="SecondDrill" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>First</t>
   </si>
@@ -158,12 +159,127 @@
   </si>
   <si>
     <t>https://exceljet.net/functions/trimrange-function#example-trimming-a-large-range</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Beds</t>
+  </si>
+  <si>
+    <t>Baths</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>5335 Lake Rd</t>
+  </si>
+  <si>
+    <t>2,003 For sale</t>
+  </si>
+  <si>
+    <t>4349 Cedar Ln</t>
+  </si>
+  <si>
+    <t>1,207 For sale</t>
+  </si>
+  <si>
+    <t>2573 Maple Ave</t>
+  </si>
+  <si>
+    <t>3,454 sold</t>
+  </si>
+  <si>
+    <t>3773 Lake Dr</t>
+  </si>
+  <si>
+    <t>3,455 sold</t>
+  </si>
+  <si>
+    <t>1659 Main Ave</t>
+  </si>
+  <si>
+    <t>1,041 For sale</t>
+  </si>
+  <si>
+    <t>2680 Lake Ave</t>
+  </si>
+  <si>
+    <t>1,535 For sale</t>
+  </si>
+  <si>
+    <t>2386 oak Rd</t>
+  </si>
+  <si>
+    <t>1,831 For sale</t>
+  </si>
+  <si>
+    <t>2636 oak st</t>
+  </si>
+  <si>
+    <t>2,646 sold</t>
+  </si>
+  <si>
+    <t>2095 Hill Dr</t>
+  </si>
+  <si>
+    <t>2,871 Sale Pending</t>
+  </si>
+  <si>
+    <t>2441 Main Ave</t>
+  </si>
+  <si>
+    <t>2,389 For sale</t>
+  </si>
+  <si>
+    <t>1632 Lake Dr</t>
+  </si>
+  <si>
+    <t>21.58 sale pending</t>
+  </si>
+  <si>
+    <t>3390 Park st</t>
+  </si>
+  <si>
+    <t>1229 For sale</t>
+  </si>
+  <si>
+    <t>4752 Maple Ln</t>
+  </si>
+  <si>
+    <t>2605 For sale</t>
+  </si>
+  <si>
+    <t>Size (sf)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>For sale</t>
+  </si>
+  <si>
+    <t>sold</t>
+  </si>
+  <si>
+    <t>Sale Pending</t>
+  </si>
+  <si>
+    <t>sale pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -249,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,12 +381,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59996337778862885"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,9 +427,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="11"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comment" xfId="8" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -804,8 +917,8 @@
   </sheetPr>
   <dimension ref="B2:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -882,7 +995,7 @@
       <c r="J4">
         <v>27</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1132,6 +1245,373 @@
       </c>
       <c r="E14">
         <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P4" r:id="rId1" location="example-trimming-a-large-range" xr:uid="{6F8A7E42-124C-4B00-9428-FAD9C703D8D8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C23439-A150-44EE-8723-4E2CE72D955C}">
+  <dimension ref="B4:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4">
+        <f>ROWS(_xlfn.DROP(_xlfn.TRIMRANGE(B:H),1))</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3">
+        <v>535680</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4">
+        <v>423910</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6">
+        <f>VLOOKUP(K5,_xlfn.DROP(_xlfn.TRIMRANGE(B:H),1),3,0)</f>
+        <v>250047</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3">
+        <v>355068</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="3">
+        <v>473365</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3">
+        <v>349562</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3887740</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3">
+        <v>628305</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="3">
+        <v>790649</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="3">
+        <v>783209</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="3">
+        <v>229702</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15">
+        <v>341303</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>250047</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17">
+        <v>6749740</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>